<commit_message>
Added The Updated WBS
</commit_message>
<xml_diff>
--- a/Documents/AI Project WBS.xlsx
+++ b/Documents/AI Project WBS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rabab Shaddad\Dropbox\KSA_SIC_2022\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toheed Arsal\Traffic-Sign-Recognition-System-using-CNN\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C698EFFC-A15A-47E1-8560-E3FC9BD8DBB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="819" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="819" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="6" r:id="rId1"/>
     <sheet name="WBS" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="69">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,9 +48,6 @@
   </si>
   <si>
     <t>In-progress</t>
-  </si>
-  <si>
-    <t>In-progress</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -155,22 +151,6 @@
   </si>
   <si>
     <t>W4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1. Sub-title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1.1. Sub-title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.1.1.1. Sub-title</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -230,11 +210,77 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Dark_Web_Crusaders</t>
+  </si>
+  <si>
+    <t>Traffic Sign Recongition System Using CNN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Exploring Generalized Traffic Sign Dataset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shamaem </t>
+  </si>
+  <si>
+    <t>28/9/2022</t>
+  </si>
+  <si>
+    <t>2. Data Acquisition and EDA</t>
+  </si>
+  <si>
+    <t>2.1  Data Acquisition</t>
+  </si>
+  <si>
+    <t>2.2  EDA</t>
+  </si>
+  <si>
+    <t>3  Pre-Processing</t>
+  </si>
+  <si>
+    <t>3,1   Normalization</t>
+  </si>
+  <si>
+    <t>3.2  Data Augmentation</t>
+  </si>
+  <si>
+    <t>3.3 EDA after pre-processing</t>
+  </si>
+  <si>
+    <t>4  Model</t>
+  </si>
+  <si>
+    <t>4.1 Building The Model</t>
+  </si>
+  <si>
+    <t>Toheed</t>
+  </si>
+  <si>
+    <t>4.2 Training The Model</t>
+  </si>
+  <si>
+    <t>4.3 Validating The Model</t>
+  </si>
+  <si>
+    <t>4.4  Testing and Evulation</t>
+  </si>
+  <si>
+    <t>4.5 Visulaizaton and Results</t>
+  </si>
+  <si>
+    <t>5  Building Interface</t>
+  </si>
+  <si>
+    <t>Shamaem /Toheed</t>
+  </si>
+  <si>
+    <t>Delayed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -854,153 +900,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>293914</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>32657</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>587829</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>141515</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Callout: Down Arrow 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A536A4DE-F45A-4B4B-BAA9-2CFC0A8A3B26}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5791200" y="653143"/>
-          <a:ext cx="1121229" cy="696686"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrowCallout">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF0000"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>These</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> dates are illustrations</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1719942</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>97971</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>163287</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Callout: Down Arrow 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1D4BBA0-1AE5-4F7B-BAF6-29F4EFF96EEE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9851571" y="674915"/>
-          <a:ext cx="1121229" cy="696686"/>
-        </a:xfrm>
-        <a:prstGeom prst="downArrowCallout">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF0000"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>These</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> status are illustrations</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1299,7 +1198,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1309,9 +1208,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:15">
@@ -1378,11 +1277,11 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="2:15" ht="15">
+    <row r="9" spans="2:15">
       <c r="B9" s="3"/>
       <c r="C9" s="41"/>
       <c r="D9" s="41" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1396,11 +1295,11 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="2:15" ht="44.4">
+    <row r="10" spans="2:15" ht="44.25">
       <c r="B10" s="3"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1414,11 +1313,11 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="2:15" ht="44.4">
+    <row r="11" spans="2:15" ht="44.25">
       <c r="B11" s="3"/>
       <c r="C11" s="42"/>
       <c r="D11" s="42" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1448,11 +1347,11 @@
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="2:15" ht="15">
+    <row r="13" spans="2:15">
       <c r="B13" s="3"/>
       <c r="C13" s="41"/>
       <c r="D13" s="41" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1562,11 +1461,11 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="2:15" ht="9.9" customHeight="1">
+    <row r="20" spans="2:15" ht="9.9499999999999993" customHeight="1">
       <c r="B20" s="3"/>
       <c r="C20" s="43"/>
       <c r="D20" s="43" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -1580,11 +1479,11 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="2:15" ht="9.9" customHeight="1">
+    <row r="21" spans="2:15" ht="9.9499999999999993" customHeight="1">
       <c r="B21" s="3"/>
       <c r="C21" s="44"/>
       <c r="D21" s="44" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -1598,11 +1497,11 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="2:15" ht="9.9" customHeight="1">
+    <row r="22" spans="2:15" ht="9.9499999999999993" customHeight="1">
       <c r="B22" s="3"/>
       <c r="C22" s="44"/>
       <c r="D22" s="44" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -1616,11 +1515,11 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="2:15" ht="9.9" customHeight="1">
+    <row r="23" spans="2:15" ht="9.9499999999999993" customHeight="1">
       <c r="B23" s="3"/>
       <c r="C23" s="44"/>
       <c r="D23" s="44" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -1650,11 +1549,11 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="2:15" ht="15">
+    <row r="25" spans="2:15">
       <c r="B25" s="3"/>
       <c r="C25" s="45"/>
       <c r="D25" s="45" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -1668,7 +1567,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="2:15" ht="15">
+    <row r="26" spans="2:15">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="45"/>
@@ -1708,7 +1607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1718,26 +1617,26 @@
       <pane xSplit="10" ySplit="13" topLeftCell="K14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="6.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="12.109375" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="27.88671875" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="12.109375" style="34" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="30" width="6.88671875" style="1" customWidth="1"/>
-    <col min="31" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="4" width="6.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="27.85546875" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="12.140625" style="34" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="30" width="6.85546875" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="15" thickBot="1"/>
-    <row r="2" spans="2:30" ht="18" thickBot="1">
+    <row r="1" spans="2:30" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:30" ht="18.75" thickBot="1">
       <c r="B2" s="28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -1758,7 +1657,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="J4" s="35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:30" hidden="1">
@@ -1767,40 +1666,44 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="J5" s="35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="2:30" ht="15" thickBot="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:30" ht="15.75" thickBot="1">
       <c r="J6" s="35"/>
     </row>
-    <row r="7" spans="2:30" ht="15" thickBot="1">
+    <row r="7" spans="2:30" ht="15.75" thickBot="1">
       <c r="B7" s="31" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C7" s="33"/>
       <c r="D7" s="32"/>
       <c r="E7" s="39">
         <f ca="1">TODAY()</f>
-        <v>44626</v>
-      </c>
-    </row>
-    <row r="8" spans="2:30" ht="15" thickBot="1">
+        <v>44846</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" ht="15.75" thickBot="1">
       <c r="B8" s="31" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="32"/>
-      <c r="E8" s="40"/>
-    </row>
-    <row r="9" spans="2:30" ht="15" thickBot="1">
+      <c r="E8" s="40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" ht="15.75" thickBot="1">
       <c r="B9" s="31" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="32"/>
-      <c r="E9" s="40"/>
-    </row>
-    <row r="10" spans="2:30" ht="15" thickBot="1"/>
+      <c r="E9" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" ht="15.75" thickBot="1"/>
     <row r="11" spans="2:30">
       <c r="B11" s="46" t="s">
         <v>0</v>
@@ -1809,43 +1712,43 @@
       <c r="D11" s="47"/>
       <c r="E11" s="47"/>
       <c r="F11" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="47" t="s">
-        <v>10</v>
-      </c>
       <c r="H11" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="47" t="s">
+      <c r="J11" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="53" t="s">
-        <v>8</v>
-      </c>
       <c r="K11" s="50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="51"/>
       <c r="M11" s="51"/>
       <c r="N11" s="51"/>
       <c r="O11" s="52"/>
       <c r="P11" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q11" s="51"/>
       <c r="R11" s="51"/>
       <c r="S11" s="51"/>
       <c r="T11" s="52"/>
       <c r="U11" s="53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V11" s="51"/>
       <c r="W11" s="51"/>
       <c r="X11" s="51"/>
       <c r="Y11" s="52"/>
       <c r="Z11" s="53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA11" s="51"/>
       <c r="AB11" s="51"/>
@@ -1863,64 +1766,64 @@
       <c r="I12" s="49"/>
       <c r="J12" s="55"/>
       <c r="K12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="N12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="Q12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="R12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R12" s="5" t="s">
+      <c r="S12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="5" t="s">
+      <c r="T12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="T12" s="5" t="s">
+      <c r="U12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U12" s="5" t="s">
+      <c r="V12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="W12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W12" s="5" t="s">
+      <c r="X12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="Y12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y12" s="5" t="s">
+      <c r="Z12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Z12" s="5" t="s">
+      <c r="AA12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AA12" s="5" t="s">
+      <c r="AB12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB12" s="5" t="s">
+      <c r="AC12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AC12" s="5" t="s">
+      <c r="AD12" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="AD12" s="6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:30">
@@ -1996,18 +1899,20 @@
     </row>
     <row r="14" spans="2:30" ht="17.100000000000001" customHeight="1">
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="10">
-        <v>43770</v>
-      </c>
-      <c r="G14" s="10">
-        <v>43774</v>
-      </c>
-      <c r="H14" s="9"/>
+      <c r="F14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I14" s="10"/>
       <c r="J14" s="11" t="s">
         <v>1</v>
@@ -2034,15 +1939,21 @@
       <c r="AD14" s="14"/>
     </row>
     <row r="15" spans="2:30">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="B15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="9"/>
+      <c r="F15" s="10">
+        <v>44571</v>
+      </c>
+      <c r="G15" s="10">
+        <v>44630</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I15" s="10"/>
       <c r="J15" s="11" t="s">
         <v>1</v>
@@ -2070,14 +1981,20 @@
     </row>
     <row r="16" spans="2:30">
       <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="C16" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="8"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="9"/>
+      <c r="F16" s="10">
+        <v>44571</v>
+      </c>
+      <c r="G16" s="10">
+        <v>44571</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I16" s="10"/>
       <c r="J16" s="11" t="s">
         <v>1</v>
@@ -2105,14 +2022,20 @@
     </row>
     <row r="17" spans="2:30">
       <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10">
+        <v>44602</v>
+      </c>
+      <c r="G17" s="10">
+        <v>44630</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I17" s="10"/>
       <c r="J17" s="11" t="s">
         <v>1</v>
@@ -2139,16 +2062,24 @@
       <c r="AD17" s="14"/>
     </row>
     <row r="18" spans="2:30">
-      <c r="B18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="9"/>
+      <c r="F18" s="10">
+        <v>44661</v>
+      </c>
+      <c r="G18" s="10">
+        <v>44691</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I18" s="10"/>
       <c r="J18" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="8"/>
@@ -2173,15 +2104,23 @@
     </row>
     <row r="19" spans="2:30">
       <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>56</v>
+      </c>
       <c r="D19" s="8"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="9"/>
+      <c r="F19" s="10">
+        <v>44661</v>
+      </c>
+      <c r="G19" s="10">
+        <v>44661</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I19" s="10"/>
       <c r="J19" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K19" s="7"/>
       <c r="L19" s="8"/>
@@ -2206,15 +2145,23 @@
     </row>
     <row r="20" spans="2:30">
       <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>57</v>
+      </c>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="9"/>
+      <c r="F20" s="10">
+        <v>44661</v>
+      </c>
+      <c r="G20" s="10">
+        <v>44661</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I20" s="10"/>
       <c r="J20" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="8"/>
@@ -2239,15 +2186,23 @@
     </row>
     <row r="21" spans="2:30">
       <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
+      <c r="C21" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="9"/>
+      <c r="F21" s="10">
+        <v>44691</v>
+      </c>
+      <c r="G21" s="10">
+        <v>44691</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="I21" s="10"/>
       <c r="J21" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K21" s="7"/>
       <c r="L21" s="8"/>
@@ -2271,16 +2226,24 @@
       <c r="AD21" s="14"/>
     </row>
     <row r="22" spans="2:30" ht="17.100000000000001" customHeight="1">
-      <c r="B22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="9"/>
+      <c r="F22" s="10">
+        <v>44722</v>
+      </c>
+      <c r="G22" s="10">
+        <v>44844</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="I22" s="10"/>
       <c r="J22" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K22" s="7"/>
       <c r="L22" s="8"/>
@@ -2305,15 +2268,23 @@
     </row>
     <row r="23" spans="2:30">
       <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="9"/>
+      <c r="F23" s="10">
+        <v>44722</v>
+      </c>
+      <c r="G23" s="10">
+        <v>44722</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="I23" s="10"/>
       <c r="J23" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
@@ -2338,15 +2309,23 @@
     </row>
     <row r="24" spans="2:30">
       <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
+      <c r="C24" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="D24" s="8"/>
       <c r="E24" s="9"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="9"/>
+      <c r="F24" s="10">
+        <v>44752</v>
+      </c>
+      <c r="G24" s="10">
+        <v>44752</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="I24" s="10"/>
       <c r="J24" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="8"/>
@@ -2371,15 +2350,23 @@
     </row>
     <row r="25" spans="2:30">
       <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
+      <c r="C25" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="D25" s="8"/>
       <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="9"/>
+      <c r="F25" s="10">
+        <v>44783</v>
+      </c>
+      <c r="G25" s="10">
+        <v>44783</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="I25" s="10"/>
       <c r="J25" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="8"/>
@@ -2404,15 +2391,23 @@
     </row>
     <row r="26" spans="2:30">
       <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
+      <c r="C26" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="D26" s="8"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="9"/>
+      <c r="F26" s="10">
+        <v>44814</v>
+      </c>
+      <c r="G26" s="10">
+        <v>44814</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="I26" s="10"/>
       <c r="J26" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K26" s="7"/>
       <c r="L26" s="8"/>
@@ -2437,15 +2432,23 @@
     </row>
     <row r="27" spans="2:30">
       <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
+      <c r="C27" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="9"/>
+      <c r="F27" s="10">
+        <v>44844</v>
+      </c>
+      <c r="G27" s="10">
+        <v>44844</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="I27" s="10"/>
       <c r="J27" s="11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="8"/>
@@ -2469,16 +2472,24 @@
       <c r="AD27" s="14"/>
     </row>
     <row r="28" spans="2:30">
-      <c r="B28" s="7"/>
+      <c r="B28" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="9"/>
+      <c r="F28" s="10">
+        <v>44875</v>
+      </c>
+      <c r="G28" s="10">
+        <v>44905</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="I28" s="10"/>
       <c r="J28" s="11" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="8"/>
@@ -2510,9 +2521,7 @@
       <c r="G29" s="10"/>
       <c r="H29" s="9"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="11" t="s">
-        <v>3</v>
-      </c>
+      <c r="J29" s="11"/>
       <c r="K29" s="7"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
@@ -2999,7 +3008,7 @@
       <c r="AC44" s="8"/>
       <c r="AD44" s="14"/>
     </row>
-    <row r="45" spans="2:30" ht="15" thickBot="1">
+    <row r="45" spans="2:30" ht="15.75" thickBot="1">
       <c r="B45" s="22"/>
       <c r="C45" s="23"/>
       <c r="D45" s="23"/>
@@ -3044,13 +3053,12 @@
     <mergeCell ref="I11:I13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J45" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J14:J45">
       <formula1>$J$3:$J$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>